<commit_message>
added some more tests
</commit_message>
<xml_diff>
--- a/test/TestJuntos.xlsx
+++ b/test/TestJuntos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="9">
   <si>
     <t>taskrun_article_number</t>
   </si>
@@ -383,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2457,12 +2457,20 @@
         <v>1</v>
       </c>
       <c r="B76">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76">
+        <v>90</v>
       </c>
       <c r="F76">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G76">
         <v>200</v>
@@ -2477,11 +2485,20 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="C77">
+        <v>9</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>90</v>
       </c>
       <c r="F77">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G77">
         <v>200</v>
@@ -2496,11 +2513,20 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C78">
+        <v>9</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>90</v>
       </c>
       <c r="F78">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G78">
         <v>200</v>
@@ -2515,11 +2541,20 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <v>9</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>90</v>
       </c>
       <c r="F79">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G79">
         <v>200</v>
@@ -2534,11 +2569,20 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="C80">
+        <v>9</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>140</v>
       </c>
       <c r="F80">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="G80">
         <v>200</v>
@@ -2553,11 +2597,20 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="C81">
+        <v>9</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>90</v>
       </c>
       <c r="F81">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G81">
         <v>200</v>
@@ -2572,11 +2625,20 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>90</v>
       </c>
       <c r="F82">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G82">
         <v>200</v>
@@ -2591,11 +2653,20 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>90</v>
       </c>
       <c r="F83">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G83">
         <v>200</v>
@@ -2610,14 +2681,26 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>9</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84">
+        <v>90</v>
       </c>
       <c r="F84">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="G84">
         <v>200</v>
+      </c>
+      <c r="H84" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -2626,14 +2709,26 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>9</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85">
+        <v>140</v>
       </c>
       <c r="F85">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="G85">
         <v>200</v>
+      </c>
+      <c r="H85" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -2641,8 +2736,10 @@
         <v>1</v>
       </c>
       <c r="B86">
-        <f t="shared" si="3"/>
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
       </c>
       <c r="F86">
         <f t="shared" si="1"/>
@@ -2651,6 +2748,9 @@
       <c r="G86">
         <v>200</v>
       </c>
+      <c r="H86" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -2658,7 +2758,10 @@
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
       </c>
       <c r="F87">
         <f t="shared" si="1"/>
@@ -2667,6 +2770,9 @@
       <c r="G87">
         <v>200</v>
       </c>
+      <c r="H87" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -2674,7 +2780,10 @@
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
       </c>
       <c r="F88">
         <f t="shared" si="1"/>
@@ -2683,6 +2792,9 @@
       <c r="G88">
         <v>200</v>
       </c>
+      <c r="H88" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -2690,7 +2802,10 @@
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>10</v>
       </c>
       <c r="F89">
         <f t="shared" si="1"/>
@@ -2699,6 +2814,9 @@
       <c r="G89">
         <v>200</v>
       </c>
+      <c r="H89" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
@@ -2706,7 +2824,10 @@
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="C90">
+        <v>10</v>
       </c>
       <c r="F90">
         <f t="shared" si="1"/>
@@ -2715,6 +2836,9 @@
       <c r="G90">
         <v>200</v>
       </c>
+      <c r="H90" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
@@ -2722,7 +2846,10 @@
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="C91">
+        <v>10</v>
       </c>
       <c r="F91">
         <f t="shared" si="1"/>
@@ -2731,6 +2858,9 @@
       <c r="G91">
         <v>200</v>
       </c>
+      <c r="H91" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
@@ -2738,7 +2868,10 @@
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
       </c>
       <c r="F92">
         <f t="shared" si="1"/>
@@ -2747,6 +2880,9 @@
       <c r="G92">
         <v>200</v>
       </c>
+      <c r="H92" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
@@ -2754,7 +2890,10 @@
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C93">
+        <v>10</v>
       </c>
       <c r="F93">
         <f t="shared" si="1"/>
@@ -2763,6 +2902,9 @@
       <c r="G93">
         <v>200</v>
       </c>
+      <c r="H93" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
@@ -2770,7 +2912,10 @@
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
       </c>
       <c r="F94">
         <f t="shared" si="1"/>
@@ -2779,6 +2924,9 @@
       <c r="G94">
         <v>200</v>
       </c>
+      <c r="H94" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -2786,7 +2934,10 @@
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>10</v>
       </c>
       <c r="F95">
         <f t="shared" si="1"/>
@@ -2795,14 +2946,19 @@
       <c r="G95">
         <v>200</v>
       </c>
+      <c r="H95" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>1</v>
       </c>
       <c r="B96">
-        <f t="shared" si="3"/>
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>11</v>
       </c>
       <c r="F96">
         <f t="shared" si="1"/>
@@ -2811,14 +2967,20 @@
       <c r="G96">
         <v>200</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>1</v>
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="C97">
+        <v>11</v>
       </c>
       <c r="F97">
         <f t="shared" si="1"/>
@@ -2827,14 +2989,20 @@
       <c r="G97">
         <v>200</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1</v>
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <v>11</v>
       </c>
       <c r="F98">
         <f t="shared" si="1"/>
@@ -2843,14 +3011,20 @@
       <c r="G98">
         <v>200</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>1</v>
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>11</v>
       </c>
       <c r="F99">
         <f t="shared" si="1"/>
@@ -2859,14 +3033,20 @@
       <c r="G99">
         <v>200</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>1</v>
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>11</v>
       </c>
       <c r="F100">
         <f t="shared" si="1"/>
@@ -2875,14 +3055,20 @@
       <c r="G100">
         <v>200</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>1</v>
       </c>
       <c r="B101">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="C101">
+        <v>11</v>
       </c>
       <c r="F101">
         <f t="shared" ref="F101:F119" si="4">E101+20</f>
@@ -2891,14 +3077,20 @@
       <c r="G101">
         <v>200</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1</v>
       </c>
       <c r="B102">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>7</v>
+      </c>
+      <c r="C102">
+        <v>11</v>
       </c>
       <c r="F102">
         <f t="shared" si="4"/>
@@ -2907,14 +3099,20 @@
       <c r="G102">
         <v>200</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
       <c r="B103">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>8</v>
+      </c>
+      <c r="C103">
+        <v>11</v>
       </c>
       <c r="F103">
         <f t="shared" si="4"/>
@@ -2923,14 +3121,20 @@
       <c r="G103">
         <v>200</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
       <c r="B104">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>9</v>
+      </c>
+      <c r="C104">
+        <v>11</v>
       </c>
       <c r="F104">
         <f t="shared" si="4"/>
@@ -2939,14 +3143,20 @@
       <c r="G104">
         <v>200</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1</v>
       </c>
       <c r="B105">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>11</v>
       </c>
       <c r="F105">
         <f t="shared" si="4"/>
@@ -2955,14 +3165,19 @@
       <c r="G105">
         <v>200</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
       <c r="B106">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>12</v>
       </c>
       <c r="F106">
         <f t="shared" si="4"/>
@@ -2971,14 +3186,20 @@
       <c r="G106">
         <v>200</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1</v>
       </c>
       <c r="B107">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="C107">
+        <v>12</v>
       </c>
       <c r="F107">
         <f t="shared" si="4"/>
@@ -2987,14 +3208,20 @@
       <c r="G107">
         <v>200</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
       <c r="B108">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>3</v>
+      </c>
+      <c r="C108">
+        <v>12</v>
       </c>
       <c r="F108">
         <f t="shared" si="4"/>
@@ -3003,14 +3230,20 @@
       <c r="G108">
         <v>200</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1</v>
       </c>
       <c r="B109">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>4</v>
+      </c>
+      <c r="C109">
+        <v>12</v>
       </c>
       <c r="F109">
         <f t="shared" si="4"/>
@@ -3019,14 +3252,20 @@
       <c r="G109">
         <v>200</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1</v>
       </c>
       <c r="B110">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="C110">
+        <v>12</v>
       </c>
       <c r="F110">
         <f t="shared" si="4"/>
@@ -3035,14 +3274,17 @@
       <c r="G110">
         <v>200</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>1</v>
       </c>
       <c r="B111">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F111">
         <f t="shared" si="4"/>
@@ -3051,14 +3293,17 @@
       <c r="G111">
         <v>200</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>1</v>
       </c>
       <c r="B112">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F112">
         <f t="shared" si="4"/>
@@ -3067,14 +3312,17 @@
       <c r="G112">
         <v>200</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>1</v>
       </c>
       <c r="B113">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F113">
         <f t="shared" si="4"/>
@@ -3083,14 +3331,17 @@
       <c r="G113">
         <v>200</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>1</v>
       </c>
       <c r="B114">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F114">
         <f t="shared" si="4"/>
@@ -3099,14 +3350,17 @@
       <c r="G114">
         <v>200</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>1</v>
       </c>
       <c r="B115">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F115">
         <f t="shared" si="4"/>
@@ -3115,14 +3369,17 @@
       <c r="G115">
         <v>200</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1</v>
       </c>
       <c r="B116">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="F116">
         <f t="shared" si="4"/>
@@ -3131,14 +3388,17 @@
       <c r="G116">
         <v>200</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>1</v>
       </c>
       <c r="B117">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="F117">
         <f t="shared" si="4"/>
@@ -3147,14 +3407,17 @@
       <c r="G117">
         <v>200</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>1</v>
       </c>
       <c r="B118">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F118">
         <f t="shared" si="4"/>
@@ -3163,14 +3426,17 @@
       <c r="G118">
         <v>200</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H118" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1</v>
       </c>
       <c r="B119">
         <f t="shared" si="3"/>
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="F119">
         <f t="shared" si="4"/>
@@ -3179,110 +3445,113 @@
       <c r="G119">
         <v>200</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H119" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>1</v>
       </c>
       <c r="B120">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="G120">
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>1</v>
       </c>
       <c r="B121">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="G121">
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1</v>
       </c>
       <c r="B122">
         <f t="shared" si="3"/>
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="G122">
         <v>200</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>1</v>
       </c>
       <c r="B123">
         <f t="shared" si="3"/>
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G123">
         <v>200</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>1</v>
       </c>
       <c r="B124">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="G124">
         <v>200</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>1</v>
       </c>
       <c r="B125">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G125">
         <v>200</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>1</v>
       </c>
       <c r="B126">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="G126">
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>1</v>
       </c>
       <c r="B127">
         <f t="shared" si="3"/>
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="G127">
         <v>200</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>1</v>
       </c>
       <c r="B128">
         <f t="shared" si="3"/>
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="G128">
         <v>200</v>
@@ -3294,7 +3563,7 @@
       </c>
       <c r="B129">
         <f t="shared" si="3"/>
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="G129">
         <v>200</v>
@@ -3306,7 +3575,7 @@
       </c>
       <c r="B130">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="G130">
         <v>200</v>
@@ -3318,7 +3587,7 @@
       </c>
       <c r="B131">
         <f t="shared" si="3"/>
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="G131">
         <v>200</v>
@@ -3330,7 +3599,7 @@
       </c>
       <c r="B132">
         <f t="shared" si="3"/>
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="G132">
         <v>200</v>
@@ -3342,7 +3611,7 @@
       </c>
       <c r="B133">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="G133">
         <v>200</v>
@@ -3354,7 +3623,7 @@
       </c>
       <c r="B134">
         <f t="shared" si="3"/>
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="G134">
         <v>200</v>
@@ -3366,7 +3635,7 @@
       </c>
       <c r="B135">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G135">
         <v>200</v>
@@ -3378,7 +3647,7 @@
       </c>
       <c r="B136">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="G136">
         <v>200</v>
@@ -3390,7 +3659,7 @@
       </c>
       <c r="B137">
         <f t="shared" si="3"/>
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="G137">
         <v>200</v>
@@ -3402,7 +3671,7 @@
       </c>
       <c r="B138">
         <f t="shared" si="3"/>
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="G138">
         <v>200</v>
@@ -3414,7 +3683,7 @@
       </c>
       <c r="B139">
         <f t="shared" ref="B139:B202" si="5">B138+1</f>
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="G139">
         <v>200</v>
@@ -3426,7 +3695,7 @@
       </c>
       <c r="B140">
         <f t="shared" si="5"/>
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="G140">
         <v>200</v>
@@ -3438,7 +3707,7 @@
       </c>
       <c r="B141">
         <f t="shared" si="5"/>
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="G141">
         <v>200</v>
@@ -3450,7 +3719,7 @@
       </c>
       <c r="B142">
         <f t="shared" si="5"/>
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="G142">
         <v>200</v>
@@ -3462,7 +3731,7 @@
       </c>
       <c r="B143">
         <f t="shared" si="5"/>
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="G143">
         <v>200</v>
@@ -3474,7 +3743,7 @@
       </c>
       <c r="B144">
         <f t="shared" si="5"/>
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="G144">
         <v>200</v>
@@ -3486,7 +3755,7 @@
       </c>
       <c r="B145">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G145">
         <v>200</v>
@@ -3498,7 +3767,7 @@
       </c>
       <c r="B146">
         <f t="shared" si="5"/>
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="G146">
         <v>200</v>
@@ -3510,7 +3779,7 @@
       </c>
       <c r="B147">
         <f t="shared" si="5"/>
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="G147">
         <v>200</v>
@@ -3522,7 +3791,7 @@
       </c>
       <c r="B148">
         <f t="shared" si="5"/>
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="G148">
         <v>200</v>
@@ -3534,7 +3803,7 @@
       </c>
       <c r="B149">
         <f t="shared" si="5"/>
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G149">
         <v>200</v>
@@ -3546,7 +3815,7 @@
       </c>
       <c r="B150">
         <f t="shared" si="5"/>
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="G150">
         <v>200</v>
@@ -3558,7 +3827,7 @@
       </c>
       <c r="B151">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="G151">
         <v>200</v>
@@ -3570,7 +3839,7 @@
       </c>
       <c r="B152">
         <f t="shared" si="5"/>
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="G152">
         <v>200</v>
@@ -3582,7 +3851,7 @@
       </c>
       <c r="B153">
         <f t="shared" si="5"/>
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="G153">
         <v>200</v>
@@ -3594,7 +3863,7 @@
       </c>
       <c r="B154">
         <f t="shared" si="5"/>
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="G154">
         <v>200</v>
@@ -3606,7 +3875,7 @@
       </c>
       <c r="B155">
         <f t="shared" si="5"/>
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G155">
         <v>200</v>
@@ -3618,7 +3887,7 @@
       </c>
       <c r="B156">
         <f t="shared" si="5"/>
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="G156">
         <v>200</v>
@@ -3630,7 +3899,7 @@
       </c>
       <c r="B157">
         <f t="shared" si="5"/>
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="G157">
         <v>200</v>
@@ -3642,7 +3911,7 @@
       </c>
       <c r="B158">
         <f t="shared" si="5"/>
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="G158">
         <v>200</v>
@@ -3654,7 +3923,7 @@
       </c>
       <c r="B159">
         <f t="shared" si="5"/>
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="G159">
         <v>200</v>
@@ -3666,7 +3935,7 @@
       </c>
       <c r="B160">
         <f t="shared" si="5"/>
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="G160">
         <v>200</v>
@@ -3678,7 +3947,7 @@
       </c>
       <c r="B161">
         <f t="shared" si="5"/>
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="G161">
         <v>200</v>
@@ -3690,7 +3959,7 @@
       </c>
       <c r="B162">
         <f t="shared" si="5"/>
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="G162">
         <v>200</v>
@@ -3702,7 +3971,7 @@
       </c>
       <c r="B163">
         <f t="shared" si="5"/>
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="G163">
         <v>200</v>
@@ -3714,7 +3983,7 @@
       </c>
       <c r="B164">
         <f t="shared" si="5"/>
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="G164">
         <v>200</v>
@@ -3726,7 +3995,7 @@
       </c>
       <c r="B165">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="G165">
         <v>200</v>
@@ -3738,7 +4007,7 @@
       </c>
       <c r="B166">
         <f t="shared" si="5"/>
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="G166">
         <v>200</v>
@@ -3750,7 +4019,7 @@
       </c>
       <c r="B167">
         <f t="shared" si="5"/>
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="G167">
         <v>200</v>
@@ -3762,7 +4031,7 @@
       </c>
       <c r="B168">
         <f t="shared" si="5"/>
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="G168">
         <v>200</v>
@@ -3774,7 +4043,7 @@
       </c>
       <c r="B169">
         <f t="shared" si="5"/>
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="G169">
         <v>200</v>
@@ -3786,7 +4055,7 @@
       </c>
       <c r="B170">
         <f t="shared" si="5"/>
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="G170">
         <v>200</v>
@@ -3798,7 +4067,7 @@
       </c>
       <c r="B171">
         <f t="shared" si="5"/>
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="G171">
         <v>200</v>
@@ -3810,7 +4079,7 @@
       </c>
       <c r="B172">
         <f t="shared" si="5"/>
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="G172">
         <v>200</v>
@@ -3822,7 +4091,7 @@
       </c>
       <c r="B173">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="G173">
         <v>200</v>
@@ -3834,7 +4103,7 @@
       </c>
       <c r="B174">
         <f t="shared" si="5"/>
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="G174">
         <v>200</v>
@@ -3846,7 +4115,7 @@
       </c>
       <c r="B175">
         <f t="shared" si="5"/>
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="G175">
         <v>200</v>
@@ -3858,7 +4127,7 @@
       </c>
       <c r="B176">
         <f t="shared" si="5"/>
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="G176">
         <v>200</v>
@@ -3870,7 +4139,7 @@
       </c>
       <c r="B177">
         <f t="shared" si="5"/>
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="G177">
         <v>200</v>
@@ -3882,7 +4151,7 @@
       </c>
       <c r="B178">
         <f t="shared" si="5"/>
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="G178">
         <v>200</v>
@@ -3894,7 +4163,7 @@
       </c>
       <c r="B179">
         <f t="shared" si="5"/>
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="G179">
         <v>200</v>
@@ -3906,7 +4175,7 @@
       </c>
       <c r="B180">
         <f t="shared" si="5"/>
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="G180">
         <v>200</v>
@@ -3918,7 +4187,7 @@
       </c>
       <c r="B181">
         <f t="shared" si="5"/>
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="G181">
         <v>200</v>
@@ -3930,7 +4199,7 @@
       </c>
       <c r="B182">
         <f t="shared" si="5"/>
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="G182">
         <v>200</v>
@@ -3942,7 +4211,7 @@
       </c>
       <c r="B183">
         <f t="shared" si="5"/>
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="G183">
         <v>200</v>
@@ -3954,7 +4223,7 @@
       </c>
       <c r="B184">
         <f t="shared" si="5"/>
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="G184">
         <v>200</v>
@@ -3966,7 +4235,7 @@
       </c>
       <c r="B185">
         <f t="shared" si="5"/>
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="G185">
         <v>200</v>
@@ -3978,7 +4247,7 @@
       </c>
       <c r="B186">
         <f t="shared" si="5"/>
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="G186">
         <v>200</v>
@@ -3990,7 +4259,7 @@
       </c>
       <c r="B187">
         <f t="shared" si="5"/>
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="G187">
         <v>200</v>
@@ -4002,7 +4271,7 @@
       </c>
       <c r="B188">
         <f t="shared" si="5"/>
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="G188">
         <v>200</v>
@@ -4014,7 +4283,7 @@
       </c>
       <c r="B189">
         <f t="shared" si="5"/>
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="G189">
         <v>200</v>
@@ -4026,7 +4295,7 @@
       </c>
       <c r="B190">
         <f t="shared" si="5"/>
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="G190">
         <v>200</v>
@@ -4038,7 +4307,7 @@
       </c>
       <c r="B191">
         <f t="shared" si="5"/>
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="G191">
         <v>200</v>
@@ -4050,7 +4319,7 @@
       </c>
       <c r="B192">
         <f t="shared" si="5"/>
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="G192">
         <v>200</v>
@@ -4062,7 +4331,7 @@
       </c>
       <c r="B193">
         <f t="shared" si="5"/>
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="G193">
         <v>200</v>
@@ -4074,7 +4343,7 @@
       </c>
       <c r="B194">
         <f t="shared" si="5"/>
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="G194">
         <v>200</v>
@@ -4086,7 +4355,7 @@
       </c>
       <c r="B195">
         <f t="shared" si="5"/>
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="G195">
         <v>200</v>
@@ -4098,7 +4367,7 @@
       </c>
       <c r="B196">
         <f t="shared" si="5"/>
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="G196">
         <v>200</v>
@@ -4110,7 +4379,7 @@
       </c>
       <c r="B197">
         <f t="shared" si="5"/>
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="G197">
         <v>200</v>
@@ -4122,7 +4391,7 @@
       </c>
       <c r="B198">
         <f t="shared" si="5"/>
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="G198">
         <v>200</v>
@@ -4134,7 +4403,7 @@
       </c>
       <c r="B199">
         <f t="shared" si="5"/>
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="G199">
         <v>200</v>
@@ -4146,7 +4415,7 @@
       </c>
       <c r="B200">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="G200">
         <v>200</v>
@@ -4158,7 +4427,7 @@
       </c>
       <c r="B201">
         <f t="shared" si="5"/>
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="G201">
         <v>200</v>
@@ -4170,7 +4439,7 @@
       </c>
       <c r="B202">
         <f t="shared" si="5"/>
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="G202">
         <v>200</v>
@@ -4182,7 +4451,7 @@
       </c>
       <c r="B203">
         <f t="shared" ref="B203:B266" si="6">B202+1</f>
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="G203">
         <v>200</v>
@@ -4194,7 +4463,7 @@
       </c>
       <c r="B204">
         <f t="shared" si="6"/>
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="G204">
         <v>200</v>
@@ -4206,7 +4475,7 @@
       </c>
       <c r="B205">
         <f t="shared" si="6"/>
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G205">
         <v>200</v>
@@ -4218,7 +4487,7 @@
       </c>
       <c r="B206">
         <f t="shared" si="6"/>
-        <v>141</v>
+        <v>101</v>
       </c>
       <c r="G206">
         <v>200</v>
@@ -4230,7 +4499,7 @@
       </c>
       <c r="B207">
         <f t="shared" si="6"/>
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="G207">
         <v>200</v>
@@ -4242,7 +4511,7 @@
       </c>
       <c r="B208">
         <f t="shared" si="6"/>
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="G208">
         <v>200</v>
@@ -4254,7 +4523,7 @@
       </c>
       <c r="B209">
         <f t="shared" si="6"/>
-        <v>144</v>
+        <v>104</v>
       </c>
       <c r="G209">
         <v>200</v>
@@ -4266,7 +4535,7 @@
       </c>
       <c r="B210">
         <f t="shared" si="6"/>
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="G210">
         <v>200</v>
@@ -4278,7 +4547,7 @@
       </c>
       <c r="B211">
         <f t="shared" si="6"/>
-        <v>146</v>
+        <v>106</v>
       </c>
       <c r="G211">
         <v>200</v>
@@ -4290,7 +4559,7 @@
       </c>
       <c r="B212">
         <f t="shared" si="6"/>
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="G212">
         <v>200</v>
@@ -4302,7 +4571,7 @@
       </c>
       <c r="B213">
         <f t="shared" si="6"/>
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="G213">
         <v>200</v>
@@ -4314,7 +4583,7 @@
       </c>
       <c r="B214">
         <f t="shared" si="6"/>
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="G214">
         <v>200</v>
@@ -4326,7 +4595,7 @@
       </c>
       <c r="B215">
         <f t="shared" si="6"/>
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="G215">
         <v>200</v>
@@ -4338,7 +4607,7 @@
       </c>
       <c r="B216">
         <f t="shared" si="6"/>
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="G216">
         <v>200</v>
@@ -4350,7 +4619,7 @@
       </c>
       <c r="B217">
         <f t="shared" si="6"/>
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="G217">
         <v>200</v>
@@ -4362,7 +4631,7 @@
       </c>
       <c r="B218">
         <f t="shared" si="6"/>
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="G218">
         <v>200</v>
@@ -4374,7 +4643,7 @@
       </c>
       <c r="B219">
         <f t="shared" si="6"/>
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="G219">
         <v>200</v>
@@ -4386,7 +4655,7 @@
       </c>
       <c r="B220">
         <f t="shared" si="6"/>
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="G220">
         <v>200</v>
@@ -4398,7 +4667,7 @@
       </c>
       <c r="B221">
         <f t="shared" si="6"/>
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="G221">
         <v>200</v>
@@ -4410,7 +4679,7 @@
       </c>
       <c r="B222">
         <f t="shared" si="6"/>
-        <v>157</v>
+        <v>117</v>
       </c>
       <c r="G222">
         <v>200</v>
@@ -4422,7 +4691,7 @@
       </c>
       <c r="B223">
         <f t="shared" si="6"/>
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="G223">
         <v>200</v>
@@ -4434,7 +4703,7 @@
       </c>
       <c r="B224">
         <f t="shared" si="6"/>
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="G224">
         <v>200</v>
@@ -4446,7 +4715,7 @@
       </c>
       <c r="B225">
         <f t="shared" si="6"/>
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="G225">
         <v>200</v>
@@ -4458,7 +4727,7 @@
       </c>
       <c r="B226">
         <f t="shared" si="6"/>
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="G226">
         <v>200</v>
@@ -4470,7 +4739,7 @@
       </c>
       <c r="B227">
         <f t="shared" si="6"/>
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="G227">
         <v>200</v>
@@ -4482,7 +4751,7 @@
       </c>
       <c r="B228">
         <f t="shared" si="6"/>
-        <v>163</v>
+        <v>123</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -4491,7 +4760,7 @@
       </c>
       <c r="B229">
         <f t="shared" si="6"/>
-        <v>164</v>
+        <v>124</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -4500,7 +4769,7 @@
       </c>
       <c r="B230">
         <f t="shared" si="6"/>
-        <v>165</v>
+        <v>125</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -4509,7 +4778,7 @@
       </c>
       <c r="B231">
         <f t="shared" si="6"/>
-        <v>166</v>
+        <v>126</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -4518,7 +4787,7 @@
       </c>
       <c r="B232">
         <f t="shared" si="6"/>
-        <v>167</v>
+        <v>127</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -4527,7 +4796,7 @@
       </c>
       <c r="B233">
         <f t="shared" si="6"/>
-        <v>168</v>
+        <v>128</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -4536,7 +4805,7 @@
       </c>
       <c r="B234">
         <f t="shared" si="6"/>
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -4545,7 +4814,7 @@
       </c>
       <c r="B235">
         <f t="shared" si="6"/>
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -4554,7 +4823,7 @@
       </c>
       <c r="B236">
         <f t="shared" si="6"/>
-        <v>171</v>
+        <v>131</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -4563,7 +4832,7 @@
       </c>
       <c r="B237">
         <f t="shared" si="6"/>
-        <v>172</v>
+        <v>132</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -4572,7 +4841,7 @@
       </c>
       <c r="B238">
         <f t="shared" si="6"/>
-        <v>173</v>
+        <v>133</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -4581,7 +4850,7 @@
       </c>
       <c r="B239">
         <f t="shared" si="6"/>
-        <v>174</v>
+        <v>134</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -4590,7 +4859,7 @@
       </c>
       <c r="B240">
         <f t="shared" si="6"/>
-        <v>175</v>
+        <v>135</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -4599,7 +4868,7 @@
       </c>
       <c r="B241">
         <f t="shared" si="6"/>
-        <v>176</v>
+        <v>136</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
@@ -4608,7 +4877,7 @@
       </c>
       <c r="B242">
         <f t="shared" si="6"/>
-        <v>177</v>
+        <v>137</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
@@ -4617,7 +4886,7 @@
       </c>
       <c r="B243">
         <f t="shared" si="6"/>
-        <v>178</v>
+        <v>138</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -4626,7 +4895,7 @@
       </c>
       <c r="B244">
         <f t="shared" si="6"/>
-        <v>179</v>
+        <v>139</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -4635,7 +4904,7 @@
       </c>
       <c r="B245">
         <f t="shared" si="6"/>
-        <v>180</v>
+        <v>140</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -4644,7 +4913,7 @@
       </c>
       <c r="B246">
         <f t="shared" si="6"/>
-        <v>181</v>
+        <v>141</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -4653,7 +4922,7 @@
       </c>
       <c r="B247">
         <f t="shared" si="6"/>
-        <v>182</v>
+        <v>142</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -4662,7 +4931,7 @@
       </c>
       <c r="B248">
         <f t="shared" si="6"/>
-        <v>183</v>
+        <v>143</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -4671,7 +4940,7 @@
       </c>
       <c r="B249">
         <f t="shared" si="6"/>
-        <v>184</v>
+        <v>144</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -4680,7 +4949,7 @@
       </c>
       <c r="B250">
         <f t="shared" si="6"/>
-        <v>185</v>
+        <v>145</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -4689,7 +4958,7 @@
       </c>
       <c r="B251">
         <f t="shared" si="6"/>
-        <v>186</v>
+        <v>146</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -4698,7 +4967,7 @@
       </c>
       <c r="B252">
         <f t="shared" si="6"/>
-        <v>187</v>
+        <v>147</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -4707,7 +4976,7 @@
       </c>
       <c r="B253">
         <f t="shared" si="6"/>
-        <v>188</v>
+        <v>148</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -4716,7 +4985,7 @@
       </c>
       <c r="B254">
         <f t="shared" si="6"/>
-        <v>189</v>
+        <v>149</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -4725,7 +4994,7 @@
       </c>
       <c r="B255">
         <f t="shared" si="6"/>
-        <v>190</v>
+        <v>150</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -4734,7 +5003,7 @@
       </c>
       <c r="B256">
         <f t="shared" si="6"/>
-        <v>191</v>
+        <v>151</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -4743,7 +5012,7 @@
       </c>
       <c r="B257">
         <f t="shared" si="6"/>
-        <v>192</v>
+        <v>152</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -4752,7 +5021,7 @@
       </c>
       <c r="B258">
         <f t="shared" si="6"/>
-        <v>193</v>
+        <v>153</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -4761,7 +5030,7 @@
       </c>
       <c r="B259">
         <f t="shared" si="6"/>
-        <v>194</v>
+        <v>154</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -4770,7 +5039,7 @@
       </c>
       <c r="B260">
         <f t="shared" si="6"/>
-        <v>195</v>
+        <v>155</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -4779,7 +5048,7 @@
       </c>
       <c r="B261">
         <f t="shared" si="6"/>
-        <v>196</v>
+        <v>156</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -4788,7 +5057,7 @@
       </c>
       <c r="B262">
         <f t="shared" si="6"/>
-        <v>197</v>
+        <v>157</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4797,7 +5066,7 @@
       </c>
       <c r="B263">
         <f t="shared" si="6"/>
-        <v>198</v>
+        <v>158</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
@@ -4806,7 +5075,7 @@
       </c>
       <c r="B264">
         <f t="shared" si="6"/>
-        <v>199</v>
+        <v>159</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -4815,7 +5084,7 @@
       </c>
       <c r="B265">
         <f t="shared" si="6"/>
-        <v>200</v>
+        <v>160</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
@@ -4824,7 +5093,7 @@
       </c>
       <c r="B266">
         <f t="shared" si="6"/>
-        <v>201</v>
+        <v>161</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -4833,7 +5102,7 @@
       </c>
       <c r="B267">
         <f t="shared" ref="B267:B330" si="7">B266+1</f>
-        <v>202</v>
+        <v>162</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -4842,7 +5111,7 @@
       </c>
       <c r="B268">
         <f t="shared" si="7"/>
-        <v>203</v>
+        <v>163</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -4851,7 +5120,7 @@
       </c>
       <c r="B269">
         <f t="shared" si="7"/>
-        <v>204</v>
+        <v>164</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -4860,7 +5129,7 @@
       </c>
       <c r="B270">
         <f t="shared" si="7"/>
-        <v>205</v>
+        <v>165</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
@@ -4869,7 +5138,7 @@
       </c>
       <c r="B271">
         <f t="shared" si="7"/>
-        <v>206</v>
+        <v>166</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
@@ -4878,7 +5147,7 @@
       </c>
       <c r="B272">
         <f t="shared" si="7"/>
-        <v>207</v>
+        <v>167</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
@@ -4887,7 +5156,7 @@
       </c>
       <c r="B273">
         <f t="shared" si="7"/>
-        <v>208</v>
+        <v>168</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -4896,7 +5165,7 @@
       </c>
       <c r="B274">
         <f t="shared" si="7"/>
-        <v>209</v>
+        <v>169</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
@@ -4905,7 +5174,7 @@
       </c>
       <c r="B275">
         <f t="shared" si="7"/>
-        <v>210</v>
+        <v>170</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -4914,7 +5183,7 @@
       </c>
       <c r="B276">
         <f t="shared" si="7"/>
-        <v>211</v>
+        <v>171</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
@@ -4923,7 +5192,7 @@
       </c>
       <c r="B277">
         <f t="shared" si="7"/>
-        <v>212</v>
+        <v>172</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
@@ -4932,7 +5201,7 @@
       </c>
       <c r="B278">
         <f t="shared" si="7"/>
-        <v>213</v>
+        <v>173</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
@@ -4941,7 +5210,7 @@
       </c>
       <c r="B279">
         <f t="shared" si="7"/>
-        <v>214</v>
+        <v>174</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
@@ -4950,7 +5219,7 @@
       </c>
       <c r="B280">
         <f t="shared" si="7"/>
-        <v>215</v>
+        <v>175</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
@@ -4959,7 +5228,7 @@
       </c>
       <c r="B281">
         <f t="shared" si="7"/>
-        <v>216</v>
+        <v>176</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
@@ -4968,7 +5237,7 @@
       </c>
       <c r="B282">
         <f t="shared" si="7"/>
-        <v>217</v>
+        <v>177</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
@@ -4977,7 +5246,7 @@
       </c>
       <c r="B283">
         <f t="shared" si="7"/>
-        <v>218</v>
+        <v>178</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
@@ -4986,7 +5255,7 @@
       </c>
       <c r="B284">
         <f t="shared" si="7"/>
-        <v>219</v>
+        <v>179</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -4995,7 +5264,7 @@
       </c>
       <c r="B285">
         <f t="shared" si="7"/>
-        <v>220</v>
+        <v>180</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -5004,7 +5273,7 @@
       </c>
       <c r="B286">
         <f t="shared" si="7"/>
-        <v>221</v>
+        <v>181</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
@@ -5013,7 +5282,7 @@
       </c>
       <c r="B287">
         <f t="shared" si="7"/>
-        <v>222</v>
+        <v>182</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
@@ -5022,7 +5291,7 @@
       </c>
       <c r="B288">
         <f t="shared" si="7"/>
-        <v>223</v>
+        <v>183</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
@@ -5031,7 +5300,7 @@
       </c>
       <c r="B289">
         <f t="shared" si="7"/>
-        <v>224</v>
+        <v>184</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
@@ -5040,7 +5309,7 @@
       </c>
       <c r="B290">
         <f t="shared" si="7"/>
-        <v>225</v>
+        <v>185</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
@@ -5049,7 +5318,7 @@
       </c>
       <c r="B291">
         <f t="shared" si="7"/>
-        <v>226</v>
+        <v>186</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
@@ -5058,7 +5327,7 @@
       </c>
       <c r="B292">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>187</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -5067,7 +5336,7 @@
       </c>
       <c r="B293">
         <f t="shared" si="7"/>
-        <v>228</v>
+        <v>188</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
@@ -5076,7 +5345,7 @@
       </c>
       <c r="B294">
         <f t="shared" si="7"/>
-        <v>229</v>
+        <v>189</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
@@ -5085,7 +5354,7 @@
       </c>
       <c r="B295">
         <f t="shared" si="7"/>
-        <v>230</v>
+        <v>190</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
@@ -5094,7 +5363,7 @@
       </c>
       <c r="B296">
         <f t="shared" si="7"/>
-        <v>231</v>
+        <v>191</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
@@ -5103,7 +5372,7 @@
       </c>
       <c r="B297">
         <f t="shared" si="7"/>
-        <v>232</v>
+        <v>192</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
@@ -5112,7 +5381,7 @@
       </c>
       <c r="B298">
         <f t="shared" si="7"/>
-        <v>233</v>
+        <v>193</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
@@ -5121,7 +5390,7 @@
       </c>
       <c r="B299">
         <f t="shared" si="7"/>
-        <v>234</v>
+        <v>194</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
@@ -5130,7 +5399,7 @@
       </c>
       <c r="B300">
         <f t="shared" si="7"/>
-        <v>235</v>
+        <v>195</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
@@ -5139,7 +5408,7 @@
       </c>
       <c r="B301">
         <f t="shared" si="7"/>
-        <v>236</v>
+        <v>196</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
@@ -5148,7 +5417,7 @@
       </c>
       <c r="B302">
         <f t="shared" si="7"/>
-        <v>237</v>
+        <v>197</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
@@ -5157,7 +5426,7 @@
       </c>
       <c r="B303">
         <f t="shared" si="7"/>
-        <v>238</v>
+        <v>198</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
@@ -5166,7 +5435,7 @@
       </c>
       <c r="B304">
         <f t="shared" si="7"/>
-        <v>239</v>
+        <v>199</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
@@ -5175,7 +5444,7 @@
       </c>
       <c r="B305">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>200</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
@@ -5184,7 +5453,7 @@
       </c>
       <c r="B306">
         <f t="shared" si="7"/>
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
@@ -5193,7 +5462,7 @@
       </c>
       <c r="B307">
         <f t="shared" si="7"/>
-        <v>242</v>
+        <v>202</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
@@ -5202,7 +5471,7 @@
       </c>
       <c r="B308">
         <f t="shared" si="7"/>
-        <v>243</v>
+        <v>203</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
@@ -5211,7 +5480,7 @@
       </c>
       <c r="B309">
         <f t="shared" si="7"/>
-        <v>244</v>
+        <v>204</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
@@ -5220,7 +5489,7 @@
       </c>
       <c r="B310">
         <f t="shared" si="7"/>
-        <v>245</v>
+        <v>205</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
@@ -5229,7 +5498,7 @@
       </c>
       <c r="B311">
         <f t="shared" si="7"/>
-        <v>246</v>
+        <v>206</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
@@ -5238,7 +5507,7 @@
       </c>
       <c r="B312">
         <f t="shared" si="7"/>
-        <v>247</v>
+        <v>207</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
@@ -5247,7 +5516,7 @@
       </c>
       <c r="B313">
         <f t="shared" si="7"/>
-        <v>248</v>
+        <v>208</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
@@ -5256,7 +5525,7 @@
       </c>
       <c r="B314">
         <f t="shared" si="7"/>
-        <v>249</v>
+        <v>209</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
@@ -5265,7 +5534,7 @@
       </c>
       <c r="B315">
         <f t="shared" si="7"/>
-        <v>250</v>
+        <v>210</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
@@ -5274,7 +5543,7 @@
       </c>
       <c r="B316">
         <f t="shared" si="7"/>
-        <v>251</v>
+        <v>211</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
@@ -5283,7 +5552,7 @@
       </c>
       <c r="B317">
         <f t="shared" si="7"/>
-        <v>252</v>
+        <v>212</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
@@ -5292,7 +5561,7 @@
       </c>
       <c r="B318">
         <f t="shared" si="7"/>
-        <v>253</v>
+        <v>213</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
@@ -5301,7 +5570,7 @@
       </c>
       <c r="B319">
         <f t="shared" si="7"/>
-        <v>254</v>
+        <v>214</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
@@ -5310,7 +5579,7 @@
       </c>
       <c r="B320">
         <f t="shared" si="7"/>
-        <v>255</v>
+        <v>215</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
@@ -5319,7 +5588,7 @@
       </c>
       <c r="B321">
         <f t="shared" si="7"/>
-        <v>256</v>
+        <v>216</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
@@ -5328,7 +5597,7 @@
       </c>
       <c r="B322">
         <f t="shared" si="7"/>
-        <v>257</v>
+        <v>217</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
@@ -5337,7 +5606,7 @@
       </c>
       <c r="B323">
         <f t="shared" si="7"/>
-        <v>258</v>
+        <v>218</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
@@ -5346,7 +5615,7 @@
       </c>
       <c r="B324">
         <f t="shared" si="7"/>
-        <v>259</v>
+        <v>219</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
@@ -5355,7 +5624,7 @@
       </c>
       <c r="B325">
         <f t="shared" si="7"/>
-        <v>260</v>
+        <v>220</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
@@ -5364,7 +5633,7 @@
       </c>
       <c r="B326">
         <f t="shared" si="7"/>
-        <v>261</v>
+        <v>221</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
@@ -5373,7 +5642,7 @@
       </c>
       <c r="B327">
         <f t="shared" si="7"/>
-        <v>262</v>
+        <v>222</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
@@ -5382,7 +5651,7 @@
       </c>
       <c r="B328">
         <f t="shared" si="7"/>
-        <v>263</v>
+        <v>223</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
@@ -5391,7 +5660,7 @@
       </c>
       <c r="B329">
         <f t="shared" si="7"/>
-        <v>264</v>
+        <v>224</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
@@ -5400,7 +5669,7 @@
       </c>
       <c r="B330">
         <f t="shared" si="7"/>
-        <v>265</v>
+        <v>225</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
@@ -5409,7 +5678,7 @@
       </c>
       <c r="B331">
         <f t="shared" ref="B331:B339" si="8">B330+1</f>
-        <v>266</v>
+        <v>226</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
@@ -5418,7 +5687,7 @@
       </c>
       <c r="B332">
         <f t="shared" si="8"/>
-        <v>267</v>
+        <v>227</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
@@ -5427,7 +5696,7 @@
       </c>
       <c r="B333">
         <f t="shared" si="8"/>
-        <v>268</v>
+        <v>228</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
@@ -5436,7 +5705,7 @@
       </c>
       <c r="B334">
         <f t="shared" si="8"/>
-        <v>269</v>
+        <v>229</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
@@ -5445,7 +5714,7 @@
       </c>
       <c r="B335">
         <f t="shared" si="8"/>
-        <v>270</v>
+        <v>230</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
@@ -5454,7 +5723,7 @@
       </c>
       <c r="B336">
         <f t="shared" si="8"/>
-        <v>271</v>
+        <v>231</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
@@ -5463,7 +5732,7 @@
       </c>
       <c r="B337">
         <f t="shared" si="8"/>
-        <v>272</v>
+        <v>232</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
@@ -5472,7 +5741,7 @@
       </c>
       <c r="B338">
         <f t="shared" si="8"/>
-        <v>273</v>
+        <v>233</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
@@ -5481,7 +5750,7 @@
       </c>
       <c r="B339">
         <f t="shared" si="8"/>
-        <v>274</v>
+        <v>234</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>